<commit_message>
azure invoice extractor sample 추가
</commit_message>
<xml_diff>
--- a/Data/Exports/invo1_1-1.xlsx
+++ b/Data/Exports/invo1_1-1.xlsx
@@ -37,123 +37,183 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
   <x:si>
+    <x:t>Name - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Name - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Vendor Address</x:t>
   </x:si>
   <x:si>
+    <x:t>Vendor Address - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Vendor Address - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Billing Name</x:t>
   </x:si>
   <x:si>
+    <x:t>Billing Name - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Billing Name - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Billing Address</x:t>
   </x:si>
   <x:si>
+    <x:t>Billing Address - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Billing Address - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Billing VAT Number</x:t>
   </x:si>
   <x:si>
+    <x:t>Billing VAT Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Billing VAT Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Shipping Address</x:t>
   </x:si>
   <x:si>
+    <x:t>Shipping Address - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Shipping Address - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Payment Address</x:t>
   </x:si>
   <x:si>
+    <x:t>Payment Address - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Payment Address - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Vendor VAT Number</x:t>
   </x:si>
   <x:si>
+    <x:t>Vendor VAT Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Vendor VAT Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Date</x:t>
   </x:si>
   <x:si>
+    <x:t>Date - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Date - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>DueDate</x:t>
   </x:si>
   <x:si>
+    <x:t>DueDate - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>DueDate - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Invoice Number</x:t>
   </x:si>
   <x:si>
+    <x:t>Invoice Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Invoice Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>PO Number</x:t>
   </x:si>
   <x:si>
+    <x:t>PO Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>PO Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Payment Terms</x:t>
   </x:si>
   <x:si>
+    <x:t>Payment Terms - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Payment Terms - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Shipping Charges</x:t>
   </x:si>
   <x:si>
+    <x:t>Shipping Charges - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Shipping Charges - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Tax Amount</x:t>
   </x:si>
   <x:si>
+    <x:t>Tax Amount - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Tax Amount - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Net Amount</x:t>
   </x:si>
   <x:si>
+    <x:t>Net Amount - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Net Amount - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Total</x:t>
   </x:si>
   <x:si>
+    <x:t>Total - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Total - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Discount</x:t>
   </x:si>
   <x:si>
+    <x:t>Discount - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Discount - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Currency</x:t>
   </x:si>
   <x:si>
+    <x:t>Currency - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Currency - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Items</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Items - Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Items - OCR Confidence</x:t>
@@ -234,42 +294,63 @@
     <x:t>Line Number</x:t>
   </x:si>
   <x:si>
+    <x:t>Line Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Line Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Description</x:t>
   </x:si>
   <x:si>
+    <x:t>Description - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Description - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Item PO Number</x:t>
   </x:si>
   <x:si>
+    <x:t>Item PO Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Item PO Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Quantity</x:t>
   </x:si>
   <x:si>
+    <x:t>Quantity - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Quantity - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Unit Price</x:t>
   </x:si>
   <x:si>
+    <x:t>Unit Price - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Unit Price - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Line Amount</x:t>
   </x:si>
   <x:si>
+    <x:t>Line Amount - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Line Amount - OCR Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Part Number</x:t>
   </x:si>
   <x:si>
+    <x:t>Part Number - Confidence</x:t>
+  </x:si>
+  <x:si>
     <x:t>Part Number - OCR Confidence</x:t>
   </x:si>
   <x:si>
@@ -318,7 +399,7 @@
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>SFP-CNB05-33709 TIP CONICAL BENT .5MM STANDARD FOR MFR-HSR Country of Origin: UNITED STATES Customer Prod: 6901000 MISC 916533</x:t>
+    <x:t>SFP-CNB05-33709 TIP CONICAL BENT.5MM STANDARD FOR MFR-HSR Country of Origin: UNITED STATES Customer Prod: 6901000 MISC 916533</x:t>
   </x:si>
   <x:si>
     <x:t>15.20</x:t>
@@ -327,7 +408,7 @@
     <x:t>30.40</x:t>
   </x:si>
   <x:si>
-    <x:t>STTC-138-33709 TIP CHISEL 1.5MM 30 DEG 700F FOR MX SYSTEMS Country of Origin: UNITED STATES</x:t>
+    <x:t>TC-138-33709 TIP CHISEL 1.5MM 30 DEG 700F FOR MX SYSTEMS Country of Origin: UNITED STATES</x:t>
   </x:si>
   <x:si>
     <x:t>23.12</x:t>
@@ -375,7 +456,7 @@
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>TT-95-50391 SOLDER TIP TINNER .70 0Z LEAD FREE RESIDUE FREE</x:t>
+    <x:t>TT-95-50391 SOLDER TIP TINNER.70 0Z LEAD FREE RESIDUE FREE</x:t>
   </x:si>
   <x:si>
     <x:t>9.90</x:t>
@@ -760,7 +841,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <x:sheetData>
-    <x:row r="1" spans="1:40" x14ac:dyDescent="0.45">
+    <x:row r="1" spans="1:60" x14ac:dyDescent="0.45">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -881,79 +962,175 @@
       <x:c r="AN1" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
+      <x:c r="AO1" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="AP1" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="AQ1" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AR1" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AS1" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="AT1" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="AU1" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AV1" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AW1" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AX1" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AY1" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AZ1" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="BA1" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="BB1" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="BC1" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="BD1" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="BE1" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="BF1" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="BG1" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="BH1" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:40" x14ac:dyDescent="0.45">
+    <x:row r="2" spans="1:60" x14ac:dyDescent="0.45">
       <x:c r="A2" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>64</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>65</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="R2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="S2" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="U2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="V2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="W2" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="X2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="Y2" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AA2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AE2" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AF2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AG2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AH2" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="AI2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AJ2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="AK2" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="AL2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="AM2" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="AN2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BC2" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="BD2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BE2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BF2" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="BG2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BH2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -979,7 +1156,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <x:sheetData>
-    <x:row r="1" spans="1:40" x14ac:dyDescent="0.45">
+    <x:row r="1" spans="1:60" x14ac:dyDescent="0.45">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1100,79 +1277,176 @@
       <x:c r="AN1" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
+      <x:c r="AO1" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="AP1" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="AQ1" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AR1" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AS1" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="AT1" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="AU1" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AV1" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AW1" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AX1" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AY1" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AZ1" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="BA1" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="BB1" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="BC1" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="BD1" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="BE1" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="BF1" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="BG1" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="BH1" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:40" customFormat="1" ht="327.75" customHeight="1" x14ac:dyDescent="0.45">
+    <x:row r="2" spans="1:60" customFormat="1" ht="327.75" customHeight="1" x14ac:dyDescent="0.45">
       <x:c r="A2" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C2" s="1" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G2" s="1" t="s">
-        <x:v>54</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J2" s="1" t="s">
+        <x:v>74</x:v>
       </x:c>
       <x:c r="K2" s="1" t="s">
-        <x:v>55</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="M2" s="1" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M2" s="1" t="s"/>
+      <x:c r="P2" s="1" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="R2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="S2" s="1" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="U2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="V2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="W2" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="X2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="Y2" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AA2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AE2" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AF2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AG2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AH2" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="AI2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AJ2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="AK2" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="AL2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="AM2" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="AN2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BC2" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="BD2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BE2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BF2" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="BG2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="BH2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1198,336 +1472,492 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <x:sheetData>
-    <x:row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A1" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="H1" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="I1" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="J1" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="K1" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="L1" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="M1" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="N1" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="O1" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="Q1" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="R1" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="S1" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="T1" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="U1" s="0" t="s">
+        <x:v>97</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A3" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L3" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="N3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P3" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="Q3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R3" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A4" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="K4" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L4" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="N4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P4" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="Q4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R4" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A5" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L5" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="N5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P5" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="Q5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R5" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A6" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L6" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="N6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P6" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="Q6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R6" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A7" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I7" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L7" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M7" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="N7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A8" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I8" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="K8" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M8" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="N8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P8" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="Q8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R8" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A9" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="H9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I9" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="K9" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M9" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="N9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P9" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="Q9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R9" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A10" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G10" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="H10" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I10" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M10" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="N10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P10" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="Q10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R10" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1551,336 +1981,492 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <x:sheetData>
-    <x:row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A1" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="H1" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="I1" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="J1" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="K1" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="L1" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="M1" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="N1" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="O1" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="Q1" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="R1" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="S1" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="T1" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="U1" s="0" t="s">
+        <x:v>97</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A3" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="N3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P3" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="Q3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A4" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
         <x:v>108</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K2" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>41</x:v>
+      <x:c r="E4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="N4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P4" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="Q4" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R4" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A3" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
+    <x:row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A5" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="N5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P5" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="Q5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A6" s="0" t="s">
         <x:v>109</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="J3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K3" s="0" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="L3" s="0" t="s">
-        <x:v>41</x:v>
+      <x:c r="B6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="N6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P6" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="Q6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R6" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A4" s="0" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="J4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K4" s="0" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="L4" s="0" t="s">
-        <x:v>41</x:v>
+    <x:row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A7" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M7" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="N7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A5" s="0" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="J5" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K5" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="L5" s="0" t="s">
-        <x:v>41</x:v>
+    <x:row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A8" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M8" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="N8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P8" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="Q8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R8" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A6" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="J6" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K6" s="0" t="s">
-        <x:v>91</x:v>
-      </x:c>
-      <x:c r="L6" s="0" t="s">
-        <x:v>41</x:v>
+    <x:row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <x:c r="A9" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="L9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M9" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="N9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P9" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="Q9" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R9" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A7" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I7" s="0" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="J7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K7" s="0" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="L7" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A8" s="0" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>112</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I8" s="0" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="J8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K8" s="0" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="L8" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <x:c r="A9" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="H9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I9" s="0" t="s">
-        <x:v>102</x:v>
-      </x:c>
-      <x:c r="J9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K9" s="0" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="L9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <x:row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <x:c r="A10" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="G10" s="0" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="H10" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="I10" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="J10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="M10" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="N10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="O10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P10" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="Q10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R10" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>